<commit_message>
Implement writing of Power_Network -> v0.1.0
Adjust Power_BusInfo and Power_Demand to fix readable name for 'i'
Fix writing of excl-values
Adjust get_dPower_BusInfo and get_dPower_Demand to include do_not_convert_values and keep_excluded_entries
Add meaningful errors to CellStyle.dict_from_xml
Implement overwriting of readableName and description for columns
Add missing changelog for Power_BusInfo and Power_Demand
</commit_message>
<xml_diff>
--- a/examples/Power_Demand.xlsx
+++ b/examples/Power_Demand.xlsx
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Node</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Node</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr">

</xml_diff>